<commit_message>
Make some changes in Scrum board and CommandFactoryMocks class.
</commit_message>
<xml_diff>
--- a/CodeSharper/Todos/Scrum-board.xlsx
+++ b/CodeSharper/Todos/Scrum-board.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\Projects\C#\CodeSharper\master\CodeSharper\Todos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -294,8 +289,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="170" formatCode="000"/>
-    <numFmt numFmtId="171" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="164" formatCode="000"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -347,13 +342,13 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -369,7 +364,24 @@
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="12">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -388,6 +400,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
@@ -406,55 +428,6 @@
         <patternFill>
           <fgColor rgb="FFFF0000"/>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="mm/dd/yy;@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="mm/dd/yy;@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode="000"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -472,16 +445,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Táblázat1" displayName="Táblázat1" ref="A1:G1048576" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Táblázat1" displayName="Táblázat1" ref="A1:G1048576" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G1048576"/>
+  <sortState ref="A2:G3">
+    <sortCondition ref="A1:A1048576"/>
+  </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" name="#" dataDxfId="11"/>
-    <tableColumn id="2" name="Priority" dataDxfId="0"/>
+    <tableColumn id="1" name="#" dataDxfId="6"/>
+    <tableColumn id="2" name="Priority" dataDxfId="5"/>
     <tableColumn id="3" name="Story" dataDxfId="4"/>
-    <tableColumn id="4" name="Description" dataDxfId="5"/>
-    <tableColumn id="5" name="Progress" dataDxfId="10"/>
-    <tableColumn id="6" name="Added" dataDxfId="9"/>
-    <tableColumn id="7" name="Completed on" dataDxfId="8"/>
+    <tableColumn id="4" name="Description" dataDxfId="3"/>
+    <tableColumn id="5" name="Progress" dataDxfId="2"/>
+    <tableColumn id="6" name="Added" dataDxfId="1"/>
+    <tableColumn id="7" name="Completed on" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -742,7 +718,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -753,7 +729,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,7 +769,6 @@
     </row>
     <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <f>ROW(A2)-1</f>
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -814,7 +789,6 @@
     </row>
     <row r="3" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <f t="shared" ref="A3:A24" si="0">ROW(A3)-1</f>
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -837,13 +811,13 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="beginsWith" dxfId="12" priority="1" operator="beginsWith" text="high">
+    <cfRule type="beginsWith" dxfId="11" priority="1" operator="beginsWith" text="high">
       <formula>LEFT(B2,LEN("high"))="high"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="14" priority="2" operator="beginsWith" text="low">
+    <cfRule type="beginsWith" dxfId="10" priority="2" operator="beginsWith" text="low">
       <formula>LEFT(B2,LEN("low"))="low"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="13" priority="3" operator="beginsWith" text="normal">
+    <cfRule type="beginsWith" dxfId="9" priority="3" operator="beginsWith" text="normal">
       <formula>LEFT(B2,LEN("normal"))="normal"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add a new task to scrum board. CodeSharper.Core/Common/ControlFlow/CommandCallControlFlow:  - Add an overloaded constructor to CommandCallControlFlow class  - Try to add a default value of Executor
</commit_message>
<xml_diff>
--- a/CodeSharper/Todos/Scrum-board.xlsx
+++ b/CodeSharper/Todos/Scrum-board.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="8130"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Description</t>
   </si>
@@ -282,6 +282,52 @@
       </rPr>
       <t>http://osherove.com/blog/2005/4/3/naming-standards-for-unit-tests.html</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Set a default </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Executor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CommandCallControlFlow</t>
+    </r>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the current version there is no option to a set default executor, so every time you have to pass an executor when a CommandCallControlFlow is initialized. I should change Executor property (set branch) visibility to public and mark it with an [Inject] attribute for supporting DI. </t>
   </si>
 </sst>
 </file>
@@ -366,6 +412,28 @@
   </cellStyles>
   <dxfs count="12">
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -408,28 +476,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -445,19 +491,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Táblázat1" displayName="Táblázat1" ref="A1:G1048576" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Táblázat1" displayName="Táblázat1" ref="A1:G1048576" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:G1048576"/>
   <sortState ref="A2:G3">
     <sortCondition ref="A1:A1048576"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" name="#" dataDxfId="6"/>
-    <tableColumn id="2" name="Priority" dataDxfId="5"/>
-    <tableColumn id="3" name="Story" dataDxfId="4"/>
-    <tableColumn id="4" name="Description" dataDxfId="3"/>
-    <tableColumn id="5" name="Progress" dataDxfId="2"/>
-    <tableColumn id="6" name="Added" dataDxfId="1"/>
-    <tableColumn id="7" name="Completed on" dataDxfId="0"/>
+    <tableColumn id="1" name="#" dataDxfId="9"/>
+    <tableColumn id="2" name="Priority" dataDxfId="8"/>
+    <tableColumn id="3" name="Story" dataDxfId="7"/>
+    <tableColumn id="4" name="Description" dataDxfId="6"/>
+    <tableColumn id="5" name="Progress" dataDxfId="5"/>
+    <tableColumn id="6" name="Added" dataDxfId="4"/>
+    <tableColumn id="7" name="Completed on" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -726,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,7 +818,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>11</v>
@@ -808,16 +854,36 @@
         <v>42004</v>
       </c>
     </row>
+    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="3">
+        <v>42004</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="beginsWith" dxfId="11" priority="1" operator="beginsWith" text="high">
+    <cfRule type="beginsWith" dxfId="2" priority="1" operator="beginsWith" text="high">
       <formula>LEFT(B2,LEN("high"))="high"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="10" priority="2" operator="beginsWith" text="low">
+    <cfRule type="beginsWith" dxfId="1" priority="2" operator="beginsWith" text="low">
       <formula>LEFT(B2,LEN("low"))="low"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="9" priority="3" operator="beginsWith" text="normal">
+    <cfRule type="beginsWith" dxfId="0" priority="3" operator="beginsWith" text="normal">
       <formula>LEFT(B2,LEN("normal"))="normal"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>